<commit_message>
Fixed CEsciFishDayRSE column name to remove extra space
</commit_message>
<xml_diff>
--- a/data-raw/RDBES Data Model CL CE.xlsx
+++ b/data-raw/RDBES Data Model CL CE.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20377"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Profile\Henrik K\Documents\GitHub\RDBES_Core_Group\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\git\icesRDBES\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60182542-F5F8-403E-A0E5-A22FB5A8DE43}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17610" windowHeight="5340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17610" windowHeight="5340" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Commercial Landing CL" sheetId="3" r:id="rId1"/>
     <sheet name="Commercial Effort CE" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1142,9 +1141,6 @@
     <t xml:space="preserve">CEscientificFishingDaysRSE </t>
   </si>
   <si>
-    <t xml:space="preserve">CEsciFishDayRSE </t>
-  </si>
-  <si>
     <t xml:space="preserve">Fishing days RSE </t>
   </si>
   <si>
@@ -1194,12 +1190,15 @@
   </si>
   <si>
     <t>Ver 1.19.4</t>
+  </si>
+  <si>
+    <t>CEsciFishDayRSE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1644,33 +1643,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="1"/>
-    <col min="3" max="3" width="15.73046875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.73046875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.86328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="1" customWidth="1"/>
     <col min="6" max="7" width="9" style="1"/>
-    <col min="8" max="8" width="12.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="41.73046875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="14.86328125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="41.7109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" style="1" customWidth="1"/>
     <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>67</v>
       </c>
@@ -1702,7 +1701,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>81</v>
       </c>
@@ -1728,7 +1727,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="11.65" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="12" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
       <c r="B3" s="8">
         <v>1</v>
@@ -1756,7 +1755,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>87</v>
       </c>
@@ -1788,7 +1787,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>87</v>
       </c>
@@ -1814,13 +1813,13 @@
         <v>6</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="J5" s="8" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>87</v>
       </c>
@@ -1852,7 +1851,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="81.400000000000006" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>87</v>
       </c>
@@ -1884,7 +1883,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>87</v>
       </c>
@@ -1916,7 +1915,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>87</v>
       </c>
@@ -1948,7 +1947,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="11.65" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="12" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>87</v>
       </c>
@@ -1980,7 +1979,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="11.65" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="12" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>87</v>
       </c>
@@ -2012,7 +2011,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="11.65" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="12" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>87</v>
       </c>
@@ -2044,7 +2043,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="81.400000000000006" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="84" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>87</v>
       </c>
@@ -2076,7 +2075,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>87</v>
       </c>
@@ -2108,7 +2107,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>87</v>
       </c>
@@ -2140,7 +2139,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>87</v>
       </c>
@@ -2172,7 +2171,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>87</v>
       </c>
@@ -2204,7 +2203,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>87</v>
       </c>
@@ -2236,7 +2235,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="11.65" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="12" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>87</v>
       </c>
@@ -2268,7 +2267,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>87</v>
       </c>
@@ -2300,7 +2299,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>87</v>
       </c>
@@ -2332,21 +2331,21 @@
         <v>261</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B22" s="8">
         <v>20</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D22" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="E22" s="8" t="s">
         <v>346</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>347</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>4</v>
@@ -2358,13 +2357,13 @@
         <v>6</v>
       </c>
       <c r="I22" s="18" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="J22" s="14" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>87</v>
       </c>
@@ -2390,13 +2389,13 @@
         <v>6</v>
       </c>
       <c r="I23" s="18" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="J23" s="7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>87</v>
       </c>
@@ -2428,7 +2427,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>87</v>
       </c>
@@ -2460,7 +2459,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>87</v>
       </c>
@@ -2492,7 +2491,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>87</v>
       </c>
@@ -2518,13 +2517,13 @@
         <v>6</v>
       </c>
       <c r="I27" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="J27" s="7" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
         <v>87</v>
       </c>
@@ -2556,7 +2555,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
         <v>87</v>
       </c>
@@ -2588,7 +2587,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
         <v>87</v>
       </c>
@@ -2620,7 +2619,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>87</v>
       </c>
@@ -2646,13 +2645,13 @@
         <v>6</v>
       </c>
       <c r="I31" s="19" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="J31" s="13" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A32" s="7"/>
       <c r="B32" s="8">
         <v>30</v>
@@ -2680,7 +2679,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A33" s="7"/>
       <c r="B33" s="8">
         <v>31</v>
@@ -2708,7 +2707,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A34" s="7"/>
       <c r="B34" s="8">
         <v>32</v>
@@ -2738,7 +2737,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="81.400000000000006" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A35" s="7"/>
       <c r="B35" s="8">
         <v>33</v>
@@ -2766,7 +2765,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A36" s="7"/>
       <c r="B36" s="8">
         <v>34</v>
@@ -2794,7 +2793,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A37" s="7"/>
       <c r="B37" s="8">
         <v>35</v>
@@ -2822,7 +2821,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A38" s="7"/>
       <c r="B38" s="8">
         <v>36</v>
@@ -2850,7 +2849,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="34.9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A39" s="7"/>
       <c r="B39" s="8">
         <v>37</v>
@@ -2874,15 +2873,15 @@
         <v>6</v>
       </c>
       <c r="I39" s="18" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="J39" s="13" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -2892,27 +2891,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="15.73046875" customWidth="1"/>
-    <col min="5" max="5" width="15.265625" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" customWidth="1"/>
-    <col min="10" max="10" width="36.86328125" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1"/>
+    <col min="10" max="10" width="36.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>67</v>
       </c>
@@ -2920,7 +2919,7 @@
         <v>39</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>38</v>
@@ -2944,7 +2943,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" ht="24" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>81</v>
       </c>
@@ -2970,7 +2969,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>87</v>
       </c>
@@ -3000,7 +2999,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="58.15" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>87</v>
       </c>
@@ -3032,7 +3031,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="46.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" ht="48" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>87</v>
       </c>
@@ -3058,13 +3057,13 @@
         <v>6</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="J5" s="8" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>87</v>
       </c>
@@ -3096,7 +3095,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="34.9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" ht="36" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>87</v>
       </c>
@@ -3128,7 +3127,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>87</v>
       </c>
@@ -3160,7 +3159,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>87</v>
       </c>
@@ -3192,7 +3191,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>87</v>
       </c>
@@ -3224,7 +3223,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="69.75" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" ht="84" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>87</v>
       </c>
@@ -3256,7 +3255,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>87</v>
       </c>
@@ -3288,7 +3287,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>87</v>
       </c>
@@ -3320,7 +3319,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="24" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>87</v>
       </c>
@@ -3352,7 +3351,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="58.15" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>87</v>
       </c>
@@ -3384,7 +3383,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="34.9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" ht="36" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>87</v>
       </c>
@@ -3410,13 +3409,13 @@
         <v>6</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="J16" s="7" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="1" customFormat="1" ht="34.9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>87</v>
       </c>
@@ -3448,7 +3447,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="46.5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" ht="48" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>87</v>
       </c>
@@ -3474,13 +3473,13 @@
         <v>6</v>
       </c>
       <c r="I18" s="18" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="J18" s="7" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="35.65" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>87</v>
       </c>
@@ -3512,7 +3511,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="35.65" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>87</v>
       </c>
@@ -3544,7 +3543,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="23.25" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>87</v>
       </c>
@@ -3576,7 +3575,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="23.25" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:11" ht="24" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>87</v>
       </c>
@@ -3602,13 +3601,13 @@
         <v>6</v>
       </c>
       <c r="I22" s="18" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="J22" s="13" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="117" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:11" ht="144.75" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" s="8">
         <v>21</v>
@@ -3636,7 +3635,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="82.15" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:11" ht="96.75" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
       <c r="B24" s="8">
         <v>22</v>
@@ -3664,7 +3663,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:11" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
       <c r="B25" s="8">
         <v>23</v>
@@ -3693,7 +3692,7 @@
       </c>
       <c r="K25" s="6"/>
     </row>
-    <row r="26" spans="1:11" ht="24" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="B26" s="8">
         <v>24</v>
@@ -3721,7 +3720,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="24" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="8">
         <v>25</v>
@@ -3749,7 +3748,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="35.65" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
       <c r="B28" s="8">
         <v>26</v>
@@ -3777,7 +3776,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="34.9" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:11" ht="36" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
       <c r="B29" s="8">
         <v>27</v>
@@ -3805,7 +3804,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="34.9" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:11" ht="36" x14ac:dyDescent="0.25">
       <c r="A30" s="9"/>
       <c r="B30" s="8">
         <v>28</v>
@@ -3833,7 +3832,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:11" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A31" s="9"/>
       <c r="B31" s="8">
         <v>29</v>
@@ -3861,7 +3860,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:11" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
       <c r="B32" s="8">
         <v>30</v>
@@ -3889,7 +3888,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:10" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
       <c r="B33" s="8">
         <v>31</v>
@@ -3917,7 +3916,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A34" s="9"/>
       <c r="B34" s="8">
         <v>32</v>
@@ -3945,7 +3944,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:10" ht="24" x14ac:dyDescent="0.25">
       <c r="A35" s="9"/>
       <c r="B35" s="8">
         <v>33</v>
@@ -3973,7 +3972,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="24" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:10" ht="36" x14ac:dyDescent="0.25">
       <c r="A36" s="9"/>
       <c r="B36" s="8">
         <v>34</v>
@@ -4001,7 +4000,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:10" ht="36" x14ac:dyDescent="0.25">
       <c r="A37" s="9"/>
       <c r="B37" s="8">
         <v>35</v>
@@ -4029,7 +4028,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="24" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:10" ht="36" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
       <c r="B38" s="8">
         <v>36</v>
@@ -4057,7 +4056,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="24" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:10" ht="36" x14ac:dyDescent="0.25">
       <c r="A39" s="9"/>
       <c r="B39" s="8">
         <v>37</v>
@@ -4085,7 +4084,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:10" ht="36" x14ac:dyDescent="0.25">
       <c r="A40" s="9"/>
       <c r="B40" s="8">
         <v>38</v>
@@ -4113,7 +4112,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:10" ht="24" x14ac:dyDescent="0.25">
       <c r="A41" s="9"/>
       <c r="B41" s="8">
         <v>39</v>
@@ -4141,7 +4140,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:10" ht="24" x14ac:dyDescent="0.25">
       <c r="A42" s="9"/>
       <c r="B42" s="8">
         <v>40</v>
@@ -4169,7 +4168,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="23.25" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:10" ht="24" x14ac:dyDescent="0.25">
       <c r="A43" s="9"/>
       <c r="B43" s="8">
         <v>41</v>
@@ -4197,7 +4196,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="34.9" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:10" ht="36" x14ac:dyDescent="0.25">
       <c r="A44" s="9"/>
       <c r="B44" s="8">
         <v>42</v>
@@ -4225,19 +4224,19 @@
         <v>213</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:10" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A45" s="9"/>
       <c r="B45" s="8">
         <v>43</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D45" s="8" t="s">
         <v>342</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>343</v>
+        <v>360</v>
       </c>
       <c r="F45" s="8" t="s">
         <v>14</v>
@@ -4253,13 +4252,13 @@
         <v>281</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="35.65" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:10" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
       <c r="B46" s="8">
         <v>44</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D46" s="8" t="s">
         <v>340</v>
@@ -4277,7 +4276,7 @@
         <v>6</v>
       </c>
       <c r="I46" s="8" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="J46" s="10" t="s">
         <v>214</v>

</xml_diff>